<commit_message>
feature: tela 2 OK! antes do gantt de capacidade
</commit_message>
<xml_diff>
--- a/src/APSSystem.Presentation.WPF/Data/Antecipacao/OrdensDeCliente.xlsx
+++ b/src/APSSystem.Presentation.WPF/Data/Antecipacao/OrdensDeCliente.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55159\source\repos\APSSystem_NOVO\src\APSSystem.Presentation.WPF\Data\Antecipacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F8B91C-07C4-4F4C-BB84-9163A03274C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99243457-BA47-4245-8E30-D570F818AD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23250" yWindow="5325" windowWidth="18180" windowHeight="9885" xr2:uid="{702DC5E7-951B-4331-8240-E292C0DE46CB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="9885" xr2:uid="{702DC5E7-951B-4331-8240-E292C0DE46CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11933,7 +11933,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:N596"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>

</xml_diff>